<commit_message>
Add title and tags on documents
</commit_message>
<xml_diff>
--- a/Documents/Mission Impossible QA Documentation.xlsx
+++ b/Documents/Mission Impossible QA Documentation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\source\repos\2223-9th-grade-sprint-math-games-mission-impossible\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\source\repos\Mission impossible\2223-9th-grade-sprint-math-games-mission-impossible\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D525DDF-6F86-4B7F-B0BF-C7AD4D68F46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Menu" sheetId="1" r:id="rId1"/>
@@ -206,7 +207,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,33 +460,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -495,6 +496,63 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -536,63 +594,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -964,20 +965,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="L16" sqref="L16:M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.36328125" customWidth="1"/>
+    <col min="14" max="14" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D1" s="18" t="s">
         <v>0</v>
       </c>
@@ -994,7 +995,7 @@
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
     </row>
-    <row r="2" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
@@ -1009,7 +1010,7 @@
       <c r="O2" s="18"/>
       <c r="P2" s="18"/>
     </row>
-    <row r="3" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
@@ -1024,7 +1025,7 @@
       <c r="O3" s="18"/>
       <c r="P3" s="18"/>
     </row>
-    <row r="4" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
@@ -1039,11 +1040,11 @@
       <c r="O4" s="18"/>
       <c r="P4" s="18"/>
     </row>
-    <row r="5" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D6" s="16" t="s">
         <v>1</v>
       </c>
@@ -1060,7 +1061,7 @@
       <c r="O6" s="16"/>
       <c r="P6" s="16"/>
     </row>
-    <row r="7" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -1075,11 +1076,11 @@
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
     </row>
-    <row r="8" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D8" s="1"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="4:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="4:16" ht="21" x14ac:dyDescent="0.5">
       <c r="D9" s="17" t="s">
         <v>2</v>
       </c>
@@ -1096,213 +1097,213 @@
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
     </row>
-    <row r="10" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D10" s="7" t="s">
+    <row r="10" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="13"/>
+      <c r="F10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="7" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="7"/>
-      <c r="L10" s="14" t="s">
+      <c r="K10" s="13"/>
+      <c r="L10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-    </row>
-    <row r="11" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
-    </row>
-    <row r="12" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D12" s="10" t="s">
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+    </row>
+    <row r="12" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="14" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="7" t="s">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="9" t="s">
+      <c r="K12" s="13"/>
+      <c r="L12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-    </row>
-    <row r="13" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-    </row>
-    <row r="14" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D14" s="1"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="4:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="D15" s="15" t="s">
+    <row r="15" spans="4:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="7" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7" t="s">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7" t="s">
+      <c r="K15" s="13"/>
+      <c r="L15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M15" s="7"/>
+      <c r="M15" s="13"/>
       <c r="N15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="P15" s="7"/>
-    </row>
-    <row r="16" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D16" s="7" t="s">
+      <c r="P15" s="13"/>
+    </row>
+    <row r="16" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8" t="s">
+      <c r="E16" s="13"/>
+      <c r="F16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8" t="s">
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8" t="s">
+      <c r="K16" s="15"/>
+      <c r="L16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8" t="s">
+      <c r="M16" s="15"/>
+      <c r="N16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="O16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P16" s="9"/>
-    </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D21" s="1"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D22" s="1"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D23" s="1"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D24" s="16" t="s">
         <v>20</v>
       </c>
@@ -1319,7 +1320,7 @@
       <c r="O24" s="16"/>
       <c r="P24" s="16"/>
     </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
@@ -1334,11 +1335,11 @@
       <c r="O25" s="16"/>
       <c r="P25" s="16"/>
     </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D26" s="1"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="4:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="27" spans="4:16" ht="21" x14ac:dyDescent="0.5">
       <c r="D27" s="17" t="s">
         <v>2</v>
       </c>
@@ -1355,213 +1356,213 @@
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
     </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D28" s="7" t="s">
+    <row r="28" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D28" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="14" t="s">
+      <c r="E28" s="13"/>
+      <c r="F28" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="7" t="s">
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K28" s="7"/>
-      <c r="L28" s="14" t="s">
+      <c r="K28" s="13"/>
+      <c r="L28" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
-      <c r="P28" s="14"/>
-    </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-    </row>
-    <row r="30" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D30" s="10" t="s">
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D30" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="14" t="s">
+      <c r="E30" s="9"/>
+      <c r="F30" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="7" t="s">
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K30" s="7"/>
-      <c r="L30" s="9" t="s">
+      <c r="K30" s="13"/>
+      <c r="L30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-    </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-    </row>
-    <row r="32" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D32" s="1"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="4:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="D33" s="15" t="s">
+    <row r="33" spans="4:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D33" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="7" t="s">
+      <c r="E33" s="14"/>
+      <c r="F33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7" t="s">
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7" t="s">
+      <c r="K33" s="13"/>
+      <c r="L33" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M33" s="7"/>
+      <c r="M33" s="13"/>
       <c r="N33" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O33" s="7" t="s">
+      <c r="O33" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="P33" s="7"/>
-    </row>
-    <row r="34" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D34" s="7" t="s">
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D34" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8" t="s">
+      <c r="E34" s="13"/>
+      <c r="F34" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8" t="s">
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8" t="s">
+      <c r="K34" s="15"/>
+      <c r="L34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8" t="s">
+      <c r="M34" s="15"/>
+      <c r="N34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O34" s="9" t="s">
+      <c r="O34" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P34" s="9"/>
-    </row>
-    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-    </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-    </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-    </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-    </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="P34" s="7"/>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D39" s="1"/>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D40" s="1"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D41" s="1"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D42" s="16" t="s">
         <v>25</v>
       </c>
@@ -1578,7 +1579,7 @@
       <c r="O42" s="16"/>
       <c r="P42" s="16"/>
     </row>
-    <row r="43" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
@@ -1593,11 +1594,11 @@
       <c r="O43" s="16"/>
       <c r="P43" s="16"/>
     </row>
-    <row r="44" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D44" s="1"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="4:16" ht="21" x14ac:dyDescent="0.4">
+    <row r="45" spans="4:16" ht="21" x14ac:dyDescent="0.5">
       <c r="D45" s="17" t="s">
         <v>2</v>
       </c>
@@ -1614,199 +1615,199 @@
       <c r="O45" s="17"/>
       <c r="P45" s="17"/>
     </row>
-    <row r="46" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D46" s="7" t="s">
+    <row r="46" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D46" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="14" t="s">
+      <c r="E46" s="13"/>
+      <c r="F46" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="7" t="s">
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="14" t="s">
+      <c r="K46" s="13"/>
+      <c r="L46" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="14"/>
-    </row>
-    <row r="47" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-    </row>
-    <row r="48" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D48" s="10" t="s">
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+    </row>
+    <row r="47" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+    </row>
+    <row r="48" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D48" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="14" t="s">
+      <c r="E48" s="9"/>
+      <c r="F48" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="7" t="s">
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K48" s="7"/>
-      <c r="L48" s="9" t="s">
+      <c r="K48" s="13"/>
+      <c r="L48" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
-    </row>
-    <row r="49" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D49" s="12"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-    </row>
-    <row r="50" spans="4:16" x14ac:dyDescent="0.3">
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+    </row>
+    <row r="50" spans="4:16" x14ac:dyDescent="0.35">
       <c r="D50" s="1"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="4:16" ht="18" x14ac:dyDescent="0.35">
-      <c r="D51" s="15" t="s">
+    <row r="51" spans="4:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D51" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="15"/>
-      <c r="F51" s="7" t="s">
+      <c r="E51" s="14"/>
+      <c r="F51" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7" t="s">
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7" t="s">
+      <c r="K51" s="13"/>
+      <c r="L51" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M51" s="7"/>
+      <c r="M51" s="13"/>
       <c r="N51" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O51" s="7" t="s">
+      <c r="O51" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="P51" s="7"/>
-    </row>
-    <row r="52" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D52" s="7" t="s">
+      <c r="P51" s="13"/>
+    </row>
+    <row r="52" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D52" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="8" t="s">
+      <c r="E52" s="13"/>
+      <c r="F52" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8" t="s">
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8" t="s">
+      <c r="K52" s="15"/>
+      <c r="L52" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="M52" s="8"/>
-      <c r="N52" s="8" t="s">
+      <c r="M52" s="15"/>
+      <c r="N52" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O52" s="9" t="s">
+      <c r="O52" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P52" s="9"/>
-    </row>
-    <row r="53" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="9"/>
-    </row>
-    <row r="54" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
-      <c r="M54" s="8"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="9"/>
-    </row>
-    <row r="55" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
-      <c r="M55" s="8"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="9"/>
-      <c r="P55" s="9"/>
-    </row>
-    <row r="56" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
-      <c r="M56" s="8"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="9"/>
+      <c r="P52" s="7"/>
+    </row>
+    <row r="53" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+    </row>
+    <row r="54" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+    </row>
+    <row r="55" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+    </row>
+    <row r="56" spans="4:16" x14ac:dyDescent="0.35">
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="15"/>
+      <c r="L56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="N56" s="15"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="64">
@@ -1880,20 +1881,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16:K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" customWidth="1"/>
+    <col min="12" max="12" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +1911,7 @@
       <c r="M1" s="53"/>
       <c r="N1" s="54"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="55"/>
       <c r="C2" s="56"/>
       <c r="D2" s="56"/>
@@ -1925,7 +1926,7 @@
       <c r="M2" s="56"/>
       <c r="N2" s="57"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="55"/>
       <c r="C3" s="56"/>
       <c r="D3" s="56"/>
@@ -1940,7 +1941,7 @@
       <c r="M3" s="56"/>
       <c r="N3" s="57"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="58"/>
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
@@ -1955,7 +1956,7 @@
       <c r="M4" s="59"/>
       <c r="N4" s="60"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -1970,7 +1971,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="61" t="s">
         <v>30</v>
       </c>
@@ -1987,7 +1988,7 @@
       <c r="M6" s="62"/>
       <c r="N6" s="63"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="64"/>
       <c r="C7" s="65"/>
       <c r="D7" s="65"/>
@@ -2002,11 +2003,11 @@
       <c r="M7" s="65"/>
       <c r="N7" s="66"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="67" t="s">
         <v>2</v>
       </c>
@@ -2023,199 +2024,199 @@
       <c r="M9" s="68"/>
       <c r="N9" s="69"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="39" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="10" t="s">
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="39" t="s">
+      <c r="I10" s="9"/>
+      <c r="J10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="41"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="44"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="27"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="39" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="10" t="s">
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="33" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="34"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="46"/>
-      <c r="N13" s="38"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="2:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="47" t="s">
+    <row r="15" spans="2:14" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="49" t="s">
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="51"/>
-      <c r="J15" s="49" t="s">
+      <c r="I15" s="37"/>
+      <c r="J15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="51"/>
+      <c r="K15" s="37"/>
       <c r="L15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="49" t="s">
+      <c r="M15" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="51"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
+      <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="21" t="s">
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="42"/>
+      <c r="J16" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="23"/>
-      <c r="L16" s="30" t="s">
+      <c r="K16" s="42"/>
+      <c r="L16" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="33" t="s">
+      <c r="M16" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="34"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="36"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="36"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="36"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="38"/>
+      <c r="N16" s="20"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B17" s="38"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="22"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="22"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B19" s="38"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="22"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2247,20 +2248,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16:K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" customWidth="1"/>
+    <col min="12" max="12" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2277,7 +2278,7 @@
       <c r="M1" s="18"/>
       <c r="N1" s="18"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2292,7 +2293,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -2307,7 +2308,7 @@
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -2322,11 +2323,11 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="16" t="s">
         <v>34</v>
       </c>
@@ -2343,7 +2344,7 @@
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -2358,11 +2359,11 @@
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="17" t="s">
         <v>2</v>
       </c>
@@ -2379,199 +2380,199 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7" t="s">
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="9" t="s">
+      <c r="I12" s="13"/>
+      <c r="J12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="2:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="2:14" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7" t="s">
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="7"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8" t="s">
+      <c r="I16" s="15"/>
+      <c r="J16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8" t="s">
+      <c r="K16" s="15"/>
+      <c r="L16" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2603,20 +2604,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16:L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" customWidth="1"/>
+    <col min="12" max="12" width="24.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2633,7 +2634,7 @@
       <c r="M1" s="18"/>
       <c r="N1" s="18"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2648,7 +2649,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -2663,7 +2664,7 @@
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -2678,11 +2679,11 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="16" t="s">
         <v>39</v>
       </c>
@@ -2699,7 +2700,7 @@
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -2714,11 +2715,11 @@
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="17" t="s">
         <v>2</v>
       </c>
@@ -2735,199 +2736,199 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="7" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="9" t="s">
+      <c r="I12" s="13"/>
+      <c r="J12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="2:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="2:14" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7" t="s">
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="7"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8" t="s">
+      <c r="I16" s="15"/>
+      <c r="J16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8" t="s">
+      <c r="K16" s="15"/>
+      <c r="L16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -2959,19 +2960,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16:L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="12" max="12" width="24.109375" customWidth="1"/>
+    <col min="12" max="12" width="24.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2988,7 +2989,7 @@
       <c r="M1" s="18"/>
       <c r="N1" s="18"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -3003,7 +3004,7 @@
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -3018,7 +3019,7 @@
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -3033,11 +3034,11 @@
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="16" t="s">
         <v>43</v>
       </c>
@@ -3054,7 +3055,7 @@
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
@@ -3069,11 +3070,11 @@
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:14" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="17" t="s">
         <v>2</v>
       </c>
@@ -3090,199 +3091,199 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="7" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="14" t="s">
+      <c r="I10" s="13"/>
+      <c r="J10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="7" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="9" t="s">
+      <c r="I12" s="13"/>
+      <c r="J12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B14" s="1"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="2:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
+    <row r="15" spans="2:14" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7" t="s">
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7" t="s">
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="7"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M15" s="7" t="s">
+      <c r="M15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="N15" s="7"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="7">
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="13">
         <v>7</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8" t="s">
+      <c r="I16" s="15"/>
+      <c r="J16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="8"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="70">
         <v>1</v>
       </c>
-      <c r="M16" s="9" t="s">
+      <c r="M16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="22">

</xml_diff>